<commit_message>
CopiarIDs, Descargar Plantilla y Subir Excel ahora son masivos, info de todos los grupos
</commit_message>
<xml_diff>
--- a/src/Plantilla Informes.xlsx
+++ b/src/Plantilla Informes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\OneDrive\Escritorio\Daniel\Congregacion Sur\Tarjetas app Dani\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC97F55-2909-4245-B01D-3A878A41FFE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E3A3D4-93B0-41DD-B1DF-C780EAD4433C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13545" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="grupo-1" sheetId="1" r:id="rId1"/>
+    <sheet name="grupo-2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -29,28 +30,17 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>DELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-No es necesario esta columna.
-El nombre no tiene que tener formato en específico.</t>
+          <t>No es necesaria esta columna.
+El nombre no tiene un formato en específico.</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{1B68AC1C-C2E7-4258-AF55-F36D2656899A}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{21C200C9-33EC-4974-890F-6D71064EFF8A}">
       <text>
         <r>
           <rPr>
@@ -60,8 +50,22 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>DELL:</t>
+          <t>Pega aquí los IDs que copiaste en la App</t>
         </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>DELL</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5E358DA0-22D4-443D-9CA4-BCC1CBE118A0}">
+      <text>
         <r>
           <rPr>
             <sz val="9"/>
@@ -69,12 +73,12 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-PRECURSOR AUXILIAR EN EL MES</t>
+          <t>No es necesaria esta columna.
+El nombre no tiene un formato en específico.</t>
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{E450184D-561B-443A-BD3D-3D74AF508427}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{76215F27-6FBC-43AC-8195-5516E41A3A2F}">
       <text>
         <r>
           <rPr>
@@ -84,17 +88,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>DELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-PRECURSOR AUXILIAR EN EL MES</t>
+          <t>Pega aquí los IDs que copiaste en la App</t>
         </r>
       </text>
     </comment>
@@ -103,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -114,42 +108,6 @@
     <t>Si</t>
   </si>
   <si>
-    <t>Enero_Participó</t>
-  </si>
-  <si>
-    <t>Enero_Estudios</t>
-  </si>
-  <si>
-    <t>Enero_Precursor</t>
-  </si>
-  <si>
-    <t>Enero_Horas</t>
-  </si>
-  <si>
-    <t>Enero_Notas</t>
-  </si>
-  <si>
-    <t>Febrero_Participó</t>
-  </si>
-  <si>
-    <t>Febrero_Estudios</t>
-  </si>
-  <si>
-    <t>Febrero_Precursor</t>
-  </si>
-  <si>
-    <t>Febrero_Horas</t>
-  </si>
-  <si>
-    <t>Febrero_Notas</t>
-  </si>
-  <si>
-    <t>enero</t>
-  </si>
-  <si>
-    <t>febrero</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -175,6 +133,57 @@
   </si>
   <si>
     <t>Pablo Gonzalez</t>
+  </si>
+  <si>
+    <t>Mes_Participó</t>
+  </si>
+  <si>
+    <t>Mes_Estudios</t>
+  </si>
+  <si>
+    <t>Mes_PrecursorAux</t>
+  </si>
+  <si>
+    <t>Mes_Horas</t>
+  </si>
+  <si>
+    <t>Mes_Notas</t>
+  </si>
+  <si>
+    <t>Septiembre_Participó</t>
+  </si>
+  <si>
+    <t>Septiembre_Estudios</t>
+  </si>
+  <si>
+    <t>Septiembre_PrecursorAux</t>
+  </si>
+  <si>
+    <t>Septiembre_Horas</t>
+  </si>
+  <si>
+    <t>Septiembre_Notas</t>
+  </si>
+  <si>
+    <t>Octubre_Participó</t>
+  </si>
+  <si>
+    <t>Octubre_Estudios</t>
+  </si>
+  <si>
+    <t>Octubre_PrecursorAux</t>
+  </si>
+  <si>
+    <t>Octubre_Horas</t>
+  </si>
+  <si>
+    <t>Octubre_Notas</t>
+  </si>
+  <si>
+    <t>Nota de Septiembre</t>
+  </si>
+  <si>
+    <t>Nota de Octubre</t>
   </si>
 </sst>
 </file>
@@ -197,11 +206,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -248,18 +256,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -268,13 +267,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,389 +775,826 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" s="2" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1">
+        <v>10</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>10</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24490112-BD1F-47D7-89EF-32B46654D761}">
+  <dimension ref="A1:Q30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="2" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
         <v>10</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="G4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1">
+        <v>10</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="I5" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3">
+      <c r="J5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1">
         <v>10</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4">
-        <v>10</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4">
-        <v>10</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="4">
-        <v>10</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="7"/>
+      <c r="L5" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="6"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="7"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="7"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="7"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="7"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="3"/>
+      <c r="A23" s="1"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>